<commit_message>
Update user interface description
</commit_message>
<xml_diff>
--- a/user interface.xlsx
+++ b/user interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BarbaraStickel\Documents\Git\gsodpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318A4C9E-AA90-4E65-A692-62200852FEDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8B3B79-1829-4F8F-9477-76ECE56C1D18}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD8043ED-C3B3-41D0-AD49-23F91994B7AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD8043ED-C3B3-41D0-AD49-23F91994B7AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Type of file</t>
   </si>
@@ -81,15 +81,9 @@
     <t>Or the uer can provide its latitude and longitude and it will download 5 closer stations</t>
   </si>
   <si>
-    <t>If TMY or Prediction is chosen</t>
-  </si>
-  <si>
     <t>IF possible only shows stations which are available in the years chosen above</t>
   </si>
   <si>
-    <t>If Historical is chosen</t>
-  </si>
-  <si>
     <t>Type of output</t>
   </si>
   <si>
@@ -100,6 +94,87 @@
   </si>
   <si>
     <t>BIN</t>
+  </si>
+  <si>
+    <t>Frequence</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>(Only if CSV or JSON)</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>If EPW:</t>
+  </si>
+  <si>
+    <t>1 file per year per location</t>
+  </si>
+  <si>
+    <t>If CSV/JSON:</t>
+  </si>
+  <si>
+    <t>65 by default</t>
+  </si>
+  <si>
+    <t>CDD temperature threshold?</t>
+  </si>
+  <si>
+    <t>HDD temperature threshold?</t>
+  </si>
+  <si>
+    <t>If Historical or TMY is chosen</t>
+  </si>
+  <si>
+    <t>If Prediction is chosen</t>
+  </si>
+  <si>
+    <t>1 file</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>HDD</t>
+  </si>
+  <si>
+    <t>CDD</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>Wind direction</t>
+  </si>
+  <si>
+    <t>Wind Speed</t>
+  </si>
+  <si>
+    <t>Data are grouped by frequency</t>
+  </si>
+  <si>
+    <t>Hourly:</t>
+  </si>
+  <si>
+    <t>Daily/Montly:</t>
+  </si>
+  <si>
+    <t>...</t>
   </si>
 </sst>
 </file>
@@ -148,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -165,22 +240,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,144 +662,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B84D70A-5F7D-4E17-9BAB-B3CC44C3F9E8}">
-  <dimension ref="B3:E29"/>
+  <dimension ref="B2:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.05078125" customWidth="1"/>
-    <col min="3" max="3" width="18.1015625" customWidth="1"/>
-    <col min="4" max="4" width="18.68359375" customWidth="1"/>
-    <col min="5" max="5" width="34.3671875" customWidth="1"/>
-    <col min="6" max="6" width="19.3671875" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="2" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="1" t="s">
+      <c r="F9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="9"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E14" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14" s="1" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F17" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="2" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="4" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="1" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="1" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E23" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="3" t="s">
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
+    </row>
+    <row r="24" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="5"/>
-      <c r="C24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="1" t="s">
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F30" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="2" t="s">
+      <c r="G30" s="11"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="4" t="s">
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>